<commit_message>
update 01 section from 10-Jul-21
</commit_message>
<xml_diff>
--- a/data/input/KTraits.xlsx
+++ b/data/input/KTraits.xlsx
@@ -3,14 +3,24 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EDE5598-4FF1-438F-AB07-8E257F8BBF02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2E6692-0BA8-4023-ADA4-DB54E52F4874}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -53,15 +63,6 @@
     <t>Max_Height</t>
   </si>
   <si>
-    <t>%C</t>
-  </si>
-  <si>
-    <t>%N</t>
-  </si>
-  <si>
-    <t>%CT</t>
-  </si>
-  <si>
     <t>LDMC_leaf</t>
   </si>
   <si>
@@ -584,25 +585,34 @@
     <t xml:space="preserve">SCO_ZEY </t>
   </si>
   <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>%P_Elsenburg</t>
-  </si>
-  <si>
-    <t>%N_UCT</t>
-  </si>
-  <si>
-    <t>%N_Elsenburg</t>
-  </si>
-  <si>
-    <t>C:N_ratio</t>
-  </si>
-  <si>
     <t>NormanI</t>
   </si>
   <si>
     <t>Wood_density</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>P_Elsenburg</t>
+  </si>
+  <si>
+    <t>N_UCT</t>
+  </si>
+  <si>
+    <t>N_Elsenburg</t>
+  </si>
+  <si>
+    <t>CN_ratio</t>
+  </si>
+  <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>species</t>
   </si>
 </sst>
 </file>
@@ -618,12 +628,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -638,13 +654,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1001,19 +1029,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomRight" activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.88671875" customWidth="1"/>
     <col min="2" max="2" width="16.5546875" customWidth="1"/>
-    <col min="14" max="16" width="13.44140625" customWidth="1"/>
-    <col min="17" max="17" width="13.77734375" customWidth="1"/>
+    <col min="14" max="14" width="10.109375" customWidth="1"/>
+    <col min="15" max="15" width="7.44140625" customWidth="1"/>
+    <col min="16" max="16" width="12" customWidth="1"/>
+    <col min="17" max="18" width="8.88671875" customWidth="1"/>
     <col min="27" max="27" width="21.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1022,7 +1052,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1043,10 +1073,10 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
+        <v>187</v>
+      </c>
+      <c r="J1" t="s">
         <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
       </c>
       <c r="K1" t="s">
         <v>9</v>
@@ -1057,58 +1087,58 @@
       <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="R1" t="s">
+        <v>191</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="U1" t="s">
+        <v>194</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="W1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
-        <v>190</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>191</v>
-      </c>
-      <c r="R1" t="s">
-        <v>192</v>
-      </c>
-      <c r="S1" t="s">
-        <v>193</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="X1" t="s">
+        <v>186</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="U1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AA1" t="s">
         <v>16</v>
       </c>
-      <c r="W1" t="s">
-        <v>194</v>
-      </c>
-      <c r="X1" t="s">
+      <c r="AB1" t="s">
         <v>17</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>195</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1129,13 +1159,13 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="J2">
-        <v>0.34899999999999998</v>
+        <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -1144,57 +1174,57 @@
         <v>30</v>
       </c>
       <c r="N2">
+        <v>0.34899999999999998</v>
+      </c>
+      <c r="O2">
         <v>47.57</v>
-      </c>
-      <c r="O2">
-        <v>2.415</v>
       </c>
       <c r="P2">
         <v>0.14000000000000001</v>
       </c>
       <c r="Q2">
+        <v>2.415</v>
+      </c>
+      <c r="R2">
         <v>2.52</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>2.31</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>18.850000000000001</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>5.7885312649999996</v>
       </c>
-      <c r="U2">
+      <c r="V2">
         <v>0.36695652200000001</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <v>12.224723539999999</v>
       </c>
-      <c r="W2">
+      <c r="X2">
         <v>11.595734370000001</v>
       </c>
-      <c r="X2">
+      <c r="Y2">
         <v>0.57499999999999996</v>
-      </c>
-      <c r="Y2">
-        <v>0.9</v>
       </c>
       <c r="Z2">
         <v>2.54</v>
       </c>
       <c r="AA2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="AB2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1215,13 +1245,13 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="J3">
-        <v>1.542</v>
+        <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="L3">
         <v>2</v>
@@ -1230,57 +1260,57 @@
         <v>8</v>
       </c>
       <c r="N3">
+        <v>1.542</v>
+      </c>
+      <c r="O3">
         <v>49.14</v>
-      </c>
-      <c r="O3">
-        <v>2.98</v>
       </c>
       <c r="P3">
         <v>0.16</v>
       </c>
       <c r="Q3">
+        <v>2.98</v>
+      </c>
+      <c r="R3">
         <v>3.13</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>2.83</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <v>15.68</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>3.3823372530000002</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <v>0.395926844</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>11.98204288</v>
       </c>
-      <c r="W3">
+      <c r="X3">
         <v>16.188831369999999</v>
       </c>
-      <c r="X3">
+      <c r="Y3">
         <v>1.4926999999999999</v>
-      </c>
-      <c r="Y3">
-        <v>0.98</v>
       </c>
       <c r="Z3">
         <v>6.9752000000000001</v>
       </c>
       <c r="AA3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="AB3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1301,13 +1331,13 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>0.77490000000000003</v>
       </c>
       <c r="J4">
-        <v>0.38200000000000001</v>
+        <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="L4">
         <v>2</v>
@@ -1316,57 +1346,57 @@
         <v>8</v>
       </c>
       <c r="N4">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="O4">
         <v>47.14</v>
-      </c>
-      <c r="O4">
-        <v>2.5299999999999998</v>
       </c>
       <c r="P4">
         <v>0.17</v>
       </c>
       <c r="Q4">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="R4">
         <v>2.8</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>2.2599999999999998</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>16.829999999999998</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>1.3133070469999999</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>0.40406320499999998</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>10.31366315</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>14.523346480000001</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <v>0.443</v>
-      </c>
-      <c r="Y4">
-        <v>0.77490000000000003</v>
       </c>
       <c r="Z4">
         <v>1.8452999999999999</v>
       </c>
       <c r="AA4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="AB4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1387,13 +1417,13 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>0.91100000000000003</v>
       </c>
       <c r="J5">
-        <v>0.19700000000000001</v>
+        <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="L5">
         <v>1</v>
@@ -1402,57 +1432,57 @@
         <v>10</v>
       </c>
       <c r="N5">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="O5">
         <v>47.28</v>
-      </c>
-      <c r="O5">
-        <v>2.75</v>
       </c>
       <c r="P5">
         <v>0.17</v>
       </c>
       <c r="Q5">
+        <v>2.75</v>
+      </c>
+      <c r="R5">
         <v>2.89</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>2.61</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>16.37</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>0.339632184</v>
       </c>
-      <c r="U5">
+      <c r="V5">
         <v>0.45289855099999998</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>8.7175728190000008</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>16.330183909999999</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
         <v>0.27600000000000002</v>
-      </c>
-      <c r="Y5">
-        <v>0.91100000000000003</v>
       </c>
       <c r="Z5">
         <v>1.1324000000000001</v>
       </c>
       <c r="AA5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="AB5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1473,13 +1503,13 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>0.68879999999999997</v>
       </c>
       <c r="J6">
-        <v>0.54500000000000004</v>
+        <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="L6">
         <v>0.83333333300000001</v>
@@ -1488,57 +1518,57 @@
         <v>15</v>
       </c>
       <c r="N6">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="O6">
         <v>48.52</v>
-      </c>
-      <c r="O6">
-        <v>2.125</v>
       </c>
       <c r="P6">
         <v>0.12</v>
       </c>
       <c r="Q6">
+        <v>2.125</v>
+      </c>
+      <c r="R6">
         <v>2.16</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>2.09</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <v>22.47</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>6.0353310630000001</v>
       </c>
-      <c r="U6">
+      <c r="V6">
         <v>0.370422535</v>
       </c>
-      <c r="V6">
+      <c r="W6">
         <v>10.0720372</v>
       </c>
-      <c r="W6">
+      <c r="X6">
         <v>9.7323344689999995</v>
       </c>
-      <c r="X6">
+      <c r="Y6">
         <v>1.42</v>
-      </c>
-      <c r="Y6">
-        <v>0.68879999999999997</v>
       </c>
       <c r="Z6">
         <v>5.2272999999999996</v>
       </c>
       <c r="AA6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="AB6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1559,13 +1589,13 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J7">
-        <v>0.40799999999999997</v>
+        <v>1</v>
       </c>
       <c r="K7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="L7">
         <v>2.6666666669999999</v>
@@ -1574,57 +1604,57 @@
         <v>20</v>
       </c>
       <c r="N7">
+        <v>0.40799999999999997</v>
+      </c>
+      <c r="O7">
         <v>44.33</v>
-      </c>
-      <c r="O7">
-        <v>2.41</v>
       </c>
       <c r="P7">
         <v>0.15</v>
       </c>
       <c r="Q7">
+        <v>2.41</v>
+      </c>
+      <c r="R7">
         <v>2.5</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>2.3199999999999998</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <v>17.71</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <v>4.2256306520000004</v>
       </c>
-      <c r="U7">
+      <c r="V7">
         <v>0.444256757</v>
       </c>
-      <c r="V7">
+      <c r="W7">
         <v>9.5297842409999998</v>
       </c>
-      <c r="W7">
+      <c r="X7">
         <v>12.347184670000001</v>
       </c>
-      <c r="X7">
+      <c r="Y7">
         <v>0.59199999999999997</v>
-      </c>
-      <c r="Y7">
-        <v>1.1000000000000001</v>
       </c>
       <c r="Z7">
         <v>2.4695999999999998</v>
       </c>
       <c r="AA7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="AB7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1645,13 +1675,13 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>0.72299999999999998</v>
       </c>
       <c r="J8">
-        <v>0.21199999999999999</v>
+        <v>1</v>
       </c>
       <c r="K8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="L8">
         <v>1.3333333329999999</v>
@@ -1660,57 +1690,57 @@
         <v>10</v>
       </c>
       <c r="N8">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="O8">
         <v>49.5</v>
-      </c>
-      <c r="O8">
-        <v>2.65</v>
       </c>
       <c r="P8">
         <v>0.19</v>
       </c>
       <c r="Q8">
+        <v>2.65</v>
+      </c>
+      <c r="R8">
         <v>2.79</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <v>2.5099999999999998</v>
       </c>
-      <c r="S8">
+      <c r="T8">
         <v>17.75</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <v>0.88310593000000004</v>
       </c>
-      <c r="U8">
+      <c r="V8">
         <v>0.36826347300000001</v>
       </c>
-      <c r="V8">
+      <c r="W8">
         <v>14.56208225</v>
       </c>
-      <c r="W8">
+      <c r="X8">
         <v>15.458447039999999</v>
       </c>
-      <c r="X8">
+      <c r="Y8">
         <v>0.33400000000000002</v>
-      </c>
-      <c r="Y8">
-        <v>0.72299999999999998</v>
       </c>
       <c r="Z8">
         <v>1.5723</v>
       </c>
       <c r="AA8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AB8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1731,13 +1761,13 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>0.73199999999999998</v>
       </c>
       <c r="J9">
-        <v>0.41899999999999998</v>
+        <v>1</v>
       </c>
       <c r="K9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="L9">
         <v>1.6666666670000001</v>
@@ -1746,57 +1776,57 @@
         <v>8</v>
       </c>
       <c r="N9">
+        <v>0.41899999999999998</v>
+      </c>
+      <c r="O9">
         <v>46.36</v>
-      </c>
-      <c r="O9">
-        <v>2.665</v>
       </c>
       <c r="P9">
         <v>0.21</v>
       </c>
       <c r="Q9">
+        <v>2.665</v>
+      </c>
+      <c r="R9">
         <v>2.75</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>2.58</v>
       </c>
-      <c r="S9">
+      <c r="T9">
         <v>16.86</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <v>1.5261583540000001</v>
       </c>
-      <c r="U9">
+      <c r="V9">
         <v>0.39891304300000002</v>
       </c>
-      <c r="V9">
+      <c r="W9">
         <v>8.964269711</v>
       </c>
-      <c r="W9">
+      <c r="X9">
         <v>15.22692082</v>
       </c>
-      <c r="X9">
+      <c r="Y9">
         <v>0.92</v>
-      </c>
-      <c r="Y9">
-        <v>0.73199999999999998</v>
       </c>
       <c r="Z9">
         <v>2.7988</v>
       </c>
       <c r="AA9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="AB9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1817,13 +1847,13 @@
         <v>1</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>0.94699999999999995</v>
       </c>
       <c r="J10">
-        <v>1.5509999999999999</v>
+        <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L10">
         <v>1.3333333329999999</v>
@@ -1832,57 +1862,57 @@
         <v>10</v>
       </c>
       <c r="N10">
+        <v>1.5509999999999999</v>
+      </c>
+      <c r="O10">
         <v>42.94</v>
-      </c>
-      <c r="O10">
-        <v>2.29</v>
       </c>
       <c r="P10">
         <v>0.15</v>
       </c>
       <c r="Q10">
+        <v>2.29</v>
+      </c>
+      <c r="R10">
         <v>2.83</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <v>1.75</v>
       </c>
-      <c r="S10">
+      <c r="T10">
         <v>15.17</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <v>1.396648291</v>
       </c>
-      <c r="U10">
+      <c r="V10">
         <v>0.33628318600000001</v>
       </c>
-      <c r="V10">
+      <c r="W10">
         <v>15.5635192</v>
       </c>
-      <c r="W10">
+      <c r="X10">
         <v>13.041675850000001</v>
       </c>
-      <c r="X10">
+      <c r="Y10">
         <v>0.45200000000000001</v>
-      </c>
-      <c r="Y10">
-        <v>0.94699999999999995</v>
       </c>
       <c r="Z10">
         <v>2.2597999999999998</v>
       </c>
       <c r="AA10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="AB10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1903,13 +1933,13 @@
         <v>1</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>0.54</v>
       </c>
       <c r="J11">
-        <v>3.8279999999999998</v>
+        <v>0</v>
       </c>
       <c r="K11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L11">
         <v>3</v>
@@ -1918,57 +1948,57 @@
         <v>10</v>
       </c>
       <c r="N11">
+        <v>3.8279999999999998</v>
+      </c>
+      <c r="O11">
         <v>42.57</v>
-      </c>
-      <c r="O11">
-        <v>2.1949999999999998</v>
       </c>
       <c r="P11">
         <v>0.15</v>
       </c>
       <c r="Q11">
+        <v>2.1949999999999998</v>
+      </c>
+      <c r="R11">
         <v>1.83</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <v>2.56</v>
       </c>
-      <c r="S11">
+      <c r="T11">
         <v>23.25</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <v>1.287980559</v>
       </c>
-      <c r="U11">
+      <c r="V11">
         <v>0.36495238099999999</v>
       </c>
-      <c r="V11">
+      <c r="W11">
         <v>13.20036737</v>
       </c>
-      <c r="W11">
+      <c r="X11">
         <v>12.526009719999999</v>
       </c>
-      <c r="X11">
+      <c r="Y11">
         <v>5.25</v>
-      </c>
-      <c r="Y11">
-        <v>0.54</v>
       </c>
       <c r="Z11">
         <v>21.098400000000002</v>
       </c>
       <c r="AA11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="AB11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1989,13 +2019,13 @@
         <v>1</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>0.84199999999999997</v>
       </c>
       <c r="J12">
-        <v>1.5549999999999999</v>
+        <v>0</v>
       </c>
       <c r="K12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L12">
         <v>0.83333333300000001</v>
@@ -2004,57 +2034,57 @@
         <v>4</v>
       </c>
       <c r="N12">
+        <v>1.5549999999999999</v>
+      </c>
+      <c r="O12">
         <v>44.39</v>
-      </c>
-      <c r="O12">
-        <v>1.68</v>
       </c>
       <c r="P12">
         <v>0.17</v>
       </c>
       <c r="Q12">
+        <v>1.68</v>
+      </c>
+      <c r="R12">
         <v>2.09</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <v>1.27</v>
       </c>
-      <c r="S12">
+      <c r="T12">
         <v>21.26</v>
       </c>
-      <c r="T12">
+      <c r="U12">
         <v>7.9052081999999996E-2</v>
       </c>
-      <c r="U12">
+      <c r="V12">
         <v>0.41265060199999998</v>
       </c>
-      <c r="V12">
+      <c r="W12">
         <v>12.279573389999999</v>
       </c>
-      <c r="W12">
+      <c r="X12">
         <v>10.04047396</v>
       </c>
-      <c r="X12">
+      <c r="Y12">
         <v>0.33200000000000002</v>
-      </c>
-      <c r="Y12">
-        <v>0.84199999999999997</v>
       </c>
       <c r="Z12">
         <v>1.6633</v>
       </c>
       <c r="AA12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="AB12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -2075,13 +2105,13 @@
         <v>1</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>0.93799999999999994</v>
       </c>
       <c r="J13">
-        <v>1.01</v>
+        <v>0</v>
       </c>
       <c r="K13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L13">
         <v>0.83333333300000001</v>
@@ -2090,57 +2120,57 @@
         <v>7</v>
       </c>
       <c r="N13">
+        <v>1.01</v>
+      </c>
+      <c r="O13">
         <v>45.38</v>
-      </c>
-      <c r="O13">
-        <v>2.3450000000000002</v>
       </c>
       <c r="P13">
         <v>0.16</v>
       </c>
       <c r="Q13">
+        <v>2.3450000000000002</v>
+      </c>
+      <c r="R13">
         <v>2.44</v>
       </c>
-      <c r="R13">
+      <c r="S13">
         <v>2.25</v>
       </c>
-      <c r="S13">
+      <c r="T13">
         <v>18.579999999999998</v>
       </c>
-      <c r="T13">
+      <c r="U13">
         <v>7.9313757999999998E-2</v>
       </c>
-      <c r="U13">
+      <c r="V13">
         <v>0.24126455899999999</v>
       </c>
-      <c r="V13">
+      <c r="W13">
         <v>21.09232497</v>
       </c>
-      <c r="W13">
+      <c r="X13">
         <v>14.03034312</v>
       </c>
-      <c r="X13">
+      <c r="Y13">
         <v>0.60099999999999998</v>
-      </c>
-      <c r="Y13">
-        <v>0.93799999999999994</v>
       </c>
       <c r="Z13">
         <v>2.9655</v>
       </c>
       <c r="AA13" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="AB13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B14" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -2161,13 +2191,13 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>0.61948950000000003</v>
       </c>
       <c r="J14">
-        <v>1.04</v>
+        <v>0</v>
       </c>
       <c r="K14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L14">
         <v>2.3333333330000001</v>
@@ -2176,57 +2206,57 @@
         <v>30</v>
       </c>
       <c r="N14">
+        <v>1.04</v>
+      </c>
+      <c r="O14">
         <v>37.49</v>
-      </c>
-      <c r="O14">
-        <v>2.9049999999999998</v>
       </c>
       <c r="P14">
         <v>0.18</v>
       </c>
       <c r="Q14">
+        <v>2.9049999999999998</v>
+      </c>
+      <c r="R14">
         <v>3</v>
       </c>
-      <c r="R14">
+      <c r="S14">
         <v>2.81</v>
       </c>
-      <c r="S14">
+      <c r="T14">
         <v>12.5</v>
       </c>
-      <c r="T14">
+      <c r="U14">
         <v>3.0411658000000001E-2</v>
       </c>
-      <c r="U14">
+      <c r="V14">
         <v>0.23930269400000001</v>
       </c>
-      <c r="V14">
+      <c r="W14">
         <v>26.12674994</v>
       </c>
-      <c r="W14">
+      <c r="X14">
         <v>17.41479417</v>
       </c>
-      <c r="X14">
+      <c r="Y14">
         <v>0.63100000000000001</v>
-      </c>
-      <c r="Y14">
-        <v>0.61948950000000003</v>
       </c>
       <c r="Z14">
         <v>3.8807999999999998</v>
       </c>
       <c r="AA14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="AB14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B15" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -2247,13 +2277,13 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="J15">
-        <v>0.32200000000000001</v>
+        <v>1</v>
       </c>
       <c r="K15" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L15">
         <v>1.3333333329999999</v>
@@ -2262,57 +2292,57 @@
         <v>13</v>
       </c>
       <c r="N15">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="O15">
         <v>38.049999999999997</v>
-      </c>
-      <c r="O15">
-        <v>2.4700000000000002</v>
       </c>
       <c r="P15">
         <v>0.17</v>
       </c>
       <c r="Q15">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="R15">
         <v>2.56</v>
       </c>
-      <c r="R15">
+      <c r="S15">
         <v>2.38</v>
       </c>
-      <c r="S15">
+      <c r="T15">
         <v>14.86</v>
       </c>
-      <c r="T15">
+      <c r="U15">
         <v>4.0148688000000002E-2</v>
       </c>
-      <c r="U15">
+      <c r="V15">
         <v>0.28246753200000002</v>
       </c>
-      <c r="V15">
+      <c r="W15">
         <v>14.301497510000001</v>
       </c>
-      <c r="W15">
+      <c r="X15">
         <v>14.79992566</v>
       </c>
-      <c r="X15">
+      <c r="Y15">
         <v>0.61599999999999999</v>
-      </c>
-      <c r="Y15">
-        <v>0.8</v>
       </c>
       <c r="Z15">
         <v>2.3675000000000002</v>
       </c>
       <c r="AA15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AB15" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B16" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -2333,13 +2363,13 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>0.75800000000000001</v>
       </c>
       <c r="J16">
-        <v>1.7210000000000001</v>
+        <v>0</v>
       </c>
       <c r="K16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L16">
         <v>1</v>
@@ -2348,57 +2378,57 @@
         <v>10</v>
       </c>
       <c r="N16">
+        <v>1.7210000000000001</v>
+      </c>
+      <c r="O16">
         <v>46.11</v>
-      </c>
-      <c r="O16">
-        <v>1.85</v>
       </c>
       <c r="P16">
         <v>0.16</v>
       </c>
       <c r="Q16">
+        <v>1.85</v>
+      </c>
+      <c r="R16">
         <v>1.95</v>
       </c>
-      <c r="R16">
+      <c r="S16">
         <v>1.75</v>
       </c>
-      <c r="S16">
+      <c r="T16">
         <v>23.7</v>
       </c>
-      <c r="T16">
+      <c r="U16">
         <v>5.2448457780000002</v>
       </c>
-      <c r="U16">
+      <c r="V16">
         <v>0.428691983</v>
       </c>
-      <c r="V16">
+      <c r="W16">
         <v>7.9586883359999998</v>
       </c>
-      <c r="W16">
+      <c r="X16">
         <v>8.4775771110000004</v>
       </c>
-      <c r="X16">
+      <c r="Y16">
         <v>1.1850000000000001</v>
-      </c>
-      <c r="Y16">
-        <v>0.75800000000000001</v>
       </c>
       <c r="Z16">
         <v>3.9184000000000001</v>
       </c>
       <c r="AA16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="AB16" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -2419,13 +2449,13 @@
         <v>0</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <v>0.72280949999999999</v>
       </c>
       <c r="J17">
-        <v>1.4359999999999999</v>
+        <v>0</v>
       </c>
       <c r="K17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L17">
         <v>1.3333333329999999</v>
@@ -2434,57 +2464,57 @@
         <v>13</v>
       </c>
       <c r="N17">
+        <v>1.4359999999999999</v>
+      </c>
+      <c r="O17">
         <v>39.880000000000003</v>
-      </c>
-      <c r="O17">
-        <v>2.95</v>
       </c>
       <c r="P17">
         <v>0.3</v>
       </c>
       <c r="Q17">
+        <v>2.95</v>
+      </c>
+      <c r="R17">
         <v>3.04</v>
       </c>
-      <c r="R17">
+      <c r="S17">
         <v>2.86</v>
       </c>
-      <c r="S17">
+      <c r="T17">
         <v>13.1</v>
       </c>
-      <c r="T17">
+      <c r="U17">
         <v>6.1127162999999998E-2</v>
       </c>
-      <c r="U17">
+      <c r="V17">
         <v>0.20538720499999999</v>
       </c>
-      <c r="V17">
+      <c r="W17">
         <v>25.433228199999999</v>
       </c>
-      <c r="W17">
+      <c r="X17">
         <v>17.66943642</v>
       </c>
-      <c r="X17">
+      <c r="Y17">
         <v>0.59399999999999997</v>
-      </c>
-      <c r="Y17">
-        <v>0.72280949999999999</v>
       </c>
       <c r="Z17">
         <v>2.4500000000000002</v>
       </c>
       <c r="AA17" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="AB17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B18" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -2505,13 +2535,13 @@
         <v>0</v>
       </c>
       <c r="I18">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="J18">
-        <v>0.89</v>
+        <v>1</v>
       </c>
       <c r="K18" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L18">
         <v>1</v>
@@ -2520,57 +2550,57 @@
         <v>6</v>
       </c>
       <c r="N18">
+        <v>0.89</v>
+      </c>
+      <c r="O18">
         <v>48.76</v>
-      </c>
-      <c r="O18">
-        <v>2.375</v>
       </c>
       <c r="P18">
         <v>0.14000000000000001</v>
       </c>
       <c r="Q18">
+        <v>2.375</v>
+      </c>
+      <c r="R18">
         <v>2.5099999999999998</v>
       </c>
-      <c r="R18">
+      <c r="S18">
         <v>2.2400000000000002</v>
       </c>
-      <c r="S18">
+      <c r="T18">
         <v>19.399999999999999</v>
       </c>
-      <c r="T18">
+      <c r="U18">
         <v>3.9615486830000002</v>
       </c>
-      <c r="U18">
+      <c r="V18">
         <v>0.37322695</v>
       </c>
-      <c r="V18">
+      <c r="W18">
         <v>11.34492251</v>
       </c>
-      <c r="W18">
+      <c r="X18">
         <v>12.26922566</v>
       </c>
-      <c r="X18">
+      <c r="Y18">
         <v>1.1279999999999999</v>
-      </c>
-      <c r="Y18">
-        <v>0.99</v>
       </c>
       <c r="Z18">
         <v>4.7187000000000001</v>
       </c>
       <c r="AA18" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="AB18" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B19" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -2591,13 +2621,13 @@
         <v>1</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="J19">
-        <v>1.2809999999999999</v>
+        <v>0</v>
       </c>
       <c r="K19" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L19">
         <v>1</v>
@@ -2606,57 +2636,57 @@
         <v>3</v>
       </c>
       <c r="N19">
+        <v>1.2809999999999999</v>
+      </c>
+      <c r="O19">
         <v>46.61</v>
-      </c>
-      <c r="O19">
-        <v>1.65</v>
       </c>
       <c r="P19">
         <v>0.13</v>
       </c>
       <c r="Q19">
+        <v>1.65</v>
+      </c>
+      <c r="R19">
         <v>1.72</v>
       </c>
-      <c r="R19">
+      <c r="S19">
         <v>1.58</v>
       </c>
-      <c r="S19">
+      <c r="T19">
         <v>27.14</v>
       </c>
-      <c r="T19">
+      <c r="U19">
         <v>0.345096236</v>
       </c>
-      <c r="U19">
+      <c r="V19">
         <v>0.34931506800000001</v>
       </c>
-      <c r="V19">
+      <c r="W19">
         <v>9.9333571430000003</v>
       </c>
-      <c r="W19">
+      <c r="X19">
         <v>9.7274518820000004</v>
       </c>
-      <c r="X19">
+      <c r="Y19">
         <v>0.14599999999999999</v>
-      </c>
-      <c r="Y19">
-        <v>0.8</v>
       </c>
       <c r="Z19">
         <v>0.51290000000000002</v>
       </c>
       <c r="AA19" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="AB19" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B20" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -2677,13 +2707,13 @@
         <v>1</v>
       </c>
       <c r="I20">
-        <v>0</v>
+        <v>0.82</v>
       </c>
       <c r="J20">
-        <v>0.42299999999999999</v>
+        <v>0</v>
       </c>
       <c r="K20" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L20">
         <v>1.3333333329999999</v>
@@ -2692,57 +2722,57 @@
         <v>10</v>
       </c>
       <c r="N20">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="O20">
         <v>44.13</v>
-      </c>
-      <c r="O20">
-        <v>2.1</v>
       </c>
       <c r="P20">
         <v>0.13</v>
       </c>
       <c r="Q20">
+        <v>2.1</v>
+      </c>
+      <c r="R20">
         <v>2.2000000000000002</v>
       </c>
-      <c r="R20">
+      <c r="S20">
         <v>2</v>
       </c>
-      <c r="S20">
+      <c r="T20">
         <v>20.09</v>
       </c>
-      <c r="T20">
+      <c r="U20">
         <v>1.237750476</v>
       </c>
-      <c r="U20">
+      <c r="V20">
         <v>0.33333333300000001</v>
       </c>
-      <c r="V20">
+      <c r="W20">
         <v>21.696666669999999</v>
       </c>
-      <c r="W20">
+      <c r="X20">
         <v>11.98112476</v>
       </c>
-      <c r="X20">
+      <c r="Y20">
         <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="Y20">
-        <v>0.82</v>
       </c>
       <c r="Z20">
         <v>0.25280000000000002</v>
       </c>
       <c r="AA20" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="AB20" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B21" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -2763,13 +2793,13 @@
         <v>1</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <v>0.77</v>
       </c>
       <c r="J21">
-        <v>0.46899999999999997</v>
+        <v>0</v>
       </c>
       <c r="K21" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L21">
         <v>3</v>
@@ -2778,57 +2808,57 @@
         <v>7</v>
       </c>
       <c r="N21">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="O21">
         <v>43.77</v>
-      </c>
-      <c r="O21">
-        <v>2.21</v>
       </c>
       <c r="P21">
         <v>0.16</v>
       </c>
       <c r="Q21">
+        <v>2.21</v>
+      </c>
+      <c r="R21">
         <v>2.3199999999999998</v>
       </c>
-      <c r="R21">
+      <c r="S21">
         <v>2.1</v>
       </c>
-      <c r="S21">
+      <c r="T21">
         <v>18.829999999999998</v>
       </c>
-      <c r="T21">
+      <c r="U21">
         <v>0.79699939099999995</v>
       </c>
-      <c r="U21">
+      <c r="V21">
         <v>0.29333333299999997</v>
       </c>
-      <c r="V21">
+      <c r="W21">
         <v>22.724</v>
       </c>
-      <c r="W21">
+      <c r="X21">
         <v>12.861500299999999</v>
       </c>
-      <c r="X21">
+      <c r="Y21">
         <v>0.15</v>
-      </c>
-      <c r="Y21">
-        <v>0.77</v>
       </c>
       <c r="Z21">
         <v>0.95009999999999994</v>
       </c>
       <c r="AA21" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="AB21" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B22" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -2849,13 +2879,13 @@
         <v>0</v>
       </c>
       <c r="I22">
-        <v>0</v>
+        <v>0.96</v>
       </c>
       <c r="J22">
-        <v>1.1619999999999999</v>
+        <v>0</v>
       </c>
       <c r="K22" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L22">
         <v>0.5</v>
@@ -2864,57 +2894,57 @@
         <v>8</v>
       </c>
       <c r="N22">
+        <v>1.1619999999999999</v>
+      </c>
+      <c r="O22">
         <v>43.55</v>
-      </c>
-      <c r="O22">
-        <v>1.85</v>
       </c>
       <c r="P22">
         <v>0.16</v>
       </c>
       <c r="Q22">
+        <v>1.85</v>
+      </c>
+      <c r="R22">
         <v>1.94</v>
       </c>
-      <c r="R22">
+      <c r="S22">
         <v>1.76</v>
       </c>
-      <c r="S22">
+      <c r="T22">
         <v>22.43</v>
       </c>
-      <c r="T22">
+      <c r="U22">
         <v>4.727958857</v>
       </c>
-      <c r="U22">
+      <c r="V22">
         <v>0.33070866100000001</v>
       </c>
-      <c r="V22">
+      <c r="W22">
         <v>11.07562182</v>
       </c>
-      <c r="W22">
+      <c r="X22">
         <v>8.7360205719999993</v>
       </c>
-      <c r="X22">
+      <c r="Y22">
         <v>1.143</v>
-      </c>
-      <c r="Y22">
-        <v>0.96</v>
       </c>
       <c r="Z22">
         <v>4.157</v>
       </c>
       <c r="AA22" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="AB22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B23" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -2935,13 +2965,13 @@
         <v>1</v>
       </c>
       <c r="I23">
-        <v>0</v>
+        <v>0.63</v>
       </c>
       <c r="J23">
-        <v>0.98499999999999999</v>
+        <v>0</v>
       </c>
       <c r="K23" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L23">
         <v>2.6666666669999999</v>
@@ -2950,57 +2980,57 @@
         <v>10</v>
       </c>
       <c r="N23">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="O23">
         <v>44.35</v>
-      </c>
-      <c r="O23">
-        <v>2.2549999999999999</v>
       </c>
       <c r="P23">
         <v>0.14000000000000001</v>
       </c>
       <c r="Q23">
+        <v>2.2549999999999999</v>
+      </c>
+      <c r="R23">
         <v>2.36</v>
       </c>
-      <c r="R23">
+      <c r="S23">
         <v>2.15</v>
       </c>
-      <c r="S23">
+      <c r="T23">
         <v>18.78</v>
       </c>
-      <c r="T23">
+      <c r="U23">
         <v>0.28741211900000002</v>
       </c>
-      <c r="U23">
+      <c r="V23">
         <v>0.40252707599999998</v>
       </c>
-      <c r="V23">
+      <c r="W23">
         <v>13.601957049999999</v>
       </c>
-      <c r="W23">
+      <c r="X23">
         <v>13.38629394</v>
       </c>
-      <c r="X23">
+      <c r="Y23">
         <v>0.55400000000000005</v>
-      </c>
-      <c r="Y23">
-        <v>0.63</v>
       </c>
       <c r="Z23">
         <v>2.9026999999999998</v>
       </c>
       <c r="AA23" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="AB23" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B24" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -3021,13 +3051,13 @@
         <v>1</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <v>0.69</v>
       </c>
       <c r="J24">
-        <v>2.25</v>
+        <v>0</v>
       </c>
       <c r="K24" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L24">
         <v>2.3333333330000001</v>
@@ -3036,57 +3066,57 @@
         <v>20</v>
       </c>
       <c r="N24">
+        <v>2.25</v>
+      </c>
+      <c r="O24">
         <v>45.84</v>
-      </c>
-      <c r="O24">
-        <v>1.76</v>
       </c>
       <c r="P24">
         <v>0.1</v>
       </c>
       <c r="Q24">
+        <v>1.76</v>
+      </c>
+      <c r="R24">
         <v>1.84</v>
       </c>
-      <c r="R24">
+      <c r="S24">
         <v>1.68</v>
       </c>
-      <c r="S24">
+      <c r="T24">
         <v>24.89</v>
       </c>
-      <c r="T24">
+      <c r="U24">
         <v>1.65931311</v>
       </c>
-      <c r="U24">
+      <c r="V24">
         <v>0.44385964900000002</v>
       </c>
-      <c r="V24">
+      <c r="W24">
         <v>11.96956634</v>
       </c>
-      <c r="W24">
+      <c r="X24">
         <v>9.7303434450000008</v>
       </c>
-      <c r="X24">
+      <c r="Y24">
         <v>0.56999999999999995</v>
-      </c>
-      <c r="Y24">
-        <v>0.69</v>
       </c>
       <c r="Z24">
         <v>2.9672999999999998</v>
       </c>
       <c r="AA24" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AB24" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B25" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -3107,13 +3137,13 @@
         <v>1</v>
       </c>
       <c r="I25">
-        <v>0</v>
+        <v>0.78400000000000003</v>
       </c>
       <c r="J25">
-        <v>0.69099999999999995</v>
+        <v>0</v>
       </c>
       <c r="K25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L25">
         <v>2.6666666669999999</v>
@@ -3122,57 +3152,57 @@
         <v>9</v>
       </c>
       <c r="N25">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="O25">
         <v>41.85</v>
-      </c>
-      <c r="O25">
-        <v>2.09</v>
       </c>
       <c r="P25">
         <v>0.1</v>
       </c>
       <c r="Q25">
+        <v>2.09</v>
+      </c>
+      <c r="R25">
         <v>2.1800000000000002</v>
       </c>
-      <c r="R25">
+      <c r="S25">
         <v>2</v>
       </c>
-      <c r="S25">
+      <c r="T25">
         <v>19.190000000000001</v>
       </c>
-      <c r="T25">
+      <c r="U25">
         <v>1.0361736130000001</v>
       </c>
-      <c r="U25">
+      <c r="V25">
         <v>0.36767849499999999</v>
       </c>
-      <c r="V25">
+      <c r="W25">
         <v>13.9877711</v>
       </c>
-      <c r="W25">
+      <c r="X25">
         <v>12.021913189999999</v>
       </c>
-      <c r="X25">
+      <c r="Y25">
         <v>0.2339</v>
-      </c>
-      <c r="Y25">
-        <v>0.78400000000000003</v>
       </c>
       <c r="Z25">
         <v>1.0978000000000001</v>
       </c>
       <c r="AA25" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="AB25" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B26" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -3193,13 +3223,13 @@
         <v>1</v>
       </c>
       <c r="I26">
-        <v>0</v>
+        <v>0.77500000000000002</v>
       </c>
       <c r="J26">
-        <v>1.3220000000000001</v>
+        <v>0</v>
       </c>
       <c r="K26" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L26">
         <v>1</v>
@@ -3208,57 +3238,57 @@
         <v>8</v>
       </c>
       <c r="N26">
+        <v>1.3220000000000001</v>
+      </c>
+      <c r="O26">
         <v>47.2</v>
-      </c>
-      <c r="O26">
-        <v>1.0900000000000001</v>
       </c>
       <c r="P26">
         <v>0.1</v>
       </c>
       <c r="Q26">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="R26">
         <v>1.1399999999999999</v>
       </c>
-      <c r="R26">
+      <c r="S26">
         <v>1.04</v>
       </c>
-      <c r="S26">
+      <c r="T26">
         <v>41.52</v>
       </c>
-      <c r="T26">
+      <c r="U26">
         <v>3.1825103119999998</v>
       </c>
-      <c r="U26">
+      <c r="V26">
         <v>0.46907216499999999</v>
       </c>
-      <c r="V26">
+      <c r="W26">
         <v>6.3413927990000003</v>
       </c>
-      <c r="W26">
+      <c r="X26">
         <v>4.9487448440000001</v>
       </c>
-      <c r="X26">
+      <c r="Y26">
         <v>0.38800000000000001</v>
-      </c>
-      <c r="Y26">
-        <v>0.77500000000000002</v>
       </c>
       <c r="Z26">
         <v>1.0721000000000001</v>
       </c>
       <c r="AA26" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="AB26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B27" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -3279,13 +3309,13 @@
         <v>1</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>0.81399999999999995</v>
       </c>
       <c r="J27">
-        <v>2.6160000000000001</v>
+        <v>0</v>
       </c>
       <c r="K27" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L27">
         <v>1.3333333329999999</v>
@@ -3294,57 +3324,57 @@
         <v>12</v>
       </c>
       <c r="N27">
+        <v>2.6160000000000001</v>
+      </c>
+      <c r="O27">
         <v>49.07</v>
-      </c>
-      <c r="O27">
-        <v>1.415</v>
       </c>
       <c r="P27">
         <v>0.1</v>
       </c>
       <c r="Q27">
+        <v>1.415</v>
+      </c>
+      <c r="R27">
         <v>1.27</v>
       </c>
-      <c r="R27">
+      <c r="S27">
         <v>1.56</v>
       </c>
-      <c r="S27">
+      <c r="T27">
         <v>38.49</v>
       </c>
-      <c r="T27">
+      <c r="U27">
         <v>3.067412241</v>
       </c>
-      <c r="U27">
+      <c r="V27">
         <v>0.493656286</v>
       </c>
-      <c r="V27">
+      <c r="W27">
         <v>6.5035020750000001</v>
       </c>
-      <c r="W27">
+      <c r="X27">
         <v>6.9562938799999996</v>
       </c>
-      <c r="X27">
+      <c r="Y27">
         <v>0.86699999999999999</v>
-      </c>
-      <c r="Y27">
-        <v>0.81399999999999995</v>
       </c>
       <c r="Z27">
         <v>2.3896000000000002</v>
       </c>
       <c r="AA27" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="AB27" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B28" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -3365,13 +3395,13 @@
         <v>1</v>
       </c>
       <c r="I28">
-        <v>0</v>
+        <v>0.63300000000000001</v>
       </c>
       <c r="J28">
-        <v>1.524</v>
+        <v>0</v>
       </c>
       <c r="K28" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L28">
         <v>1.6666666670000001</v>
@@ -3380,57 +3410,57 @@
         <v>12</v>
       </c>
       <c r="N28">
+        <v>1.524</v>
+      </c>
+      <c r="O28">
         <v>46.66</v>
-      </c>
-      <c r="O28">
-        <v>1.28</v>
       </c>
       <c r="P28">
         <v>0.13</v>
       </c>
       <c r="Q28">
+        <v>1.28</v>
+      </c>
+      <c r="R28">
         <v>1.32</v>
       </c>
-      <c r="R28">
+      <c r="S28">
         <v>1.24</v>
       </c>
-      <c r="S28">
+      <c r="T28">
         <v>35.43</v>
       </c>
-      <c r="T28">
+      <c r="U28">
         <v>3.3835978350000002</v>
       </c>
-      <c r="U28">
+      <c r="V28">
         <v>0.43197278900000002</v>
       </c>
-      <c r="V28">
+      <c r="W28">
         <v>6.4128028410000004</v>
       </c>
-      <c r="W28">
+      <c r="X28">
         <v>5.9882010829999999</v>
       </c>
-      <c r="X28">
+      <c r="Y28">
         <v>0.29399999999999998</v>
-      </c>
-      <c r="Y28">
-        <v>0.63300000000000001</v>
       </c>
       <c r="Z28">
         <v>0.78369999999999995</v>
       </c>
       <c r="AA28" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="AB28" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B29" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -3451,13 +3481,13 @@
         <v>0</v>
       </c>
       <c r="I29">
-        <v>0</v>
+        <v>0.92700000000000005</v>
       </c>
       <c r="J29">
-        <v>0.78</v>
+        <v>0</v>
       </c>
       <c r="K29" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L29">
         <v>2.3333333330000001</v>
@@ -3466,57 +3496,57 @@
         <v>5</v>
       </c>
       <c r="N29">
+        <v>0.78</v>
+      </c>
+      <c r="O29">
         <v>43</v>
-      </c>
-      <c r="O29">
-        <v>2.5550000000000002</v>
       </c>
       <c r="P29">
         <v>0.19</v>
       </c>
       <c r="Q29">
+        <v>2.5550000000000002</v>
+      </c>
+      <c r="R29">
         <v>2.66</v>
       </c>
-      <c r="R29">
+      <c r="S29">
         <v>2.4500000000000002</v>
       </c>
-      <c r="S29">
+      <c r="T29">
         <v>16.190000000000001</v>
       </c>
-      <c r="T29">
+      <c r="U29">
         <v>1.0012739859999999</v>
       </c>
-      <c r="U29">
+      <c r="V29">
         <v>0.38211382100000002</v>
       </c>
-      <c r="V29">
+      <c r="W29">
         <v>20.598749999999999</v>
       </c>
-      <c r="W29">
+      <c r="X29">
         <v>14.82936301</v>
       </c>
-      <c r="X29">
+      <c r="Y29">
         <v>0.123</v>
-      </c>
-      <c r="Y29">
-        <v>0.92700000000000005</v>
       </c>
       <c r="Z29">
         <v>0.96440000000000003</v>
       </c>
       <c r="AA29" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="AB29" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B30" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -3537,13 +3567,13 @@
         <v>1</v>
       </c>
       <c r="I30">
-        <v>1</v>
+        <v>0.66</v>
       </c>
       <c r="J30">
-        <v>1.0249999999999999</v>
+        <v>1</v>
       </c>
       <c r="K30" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L30">
         <v>0.5</v>
@@ -3552,57 +3582,57 @@
         <v>9</v>
       </c>
       <c r="N30">
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="O30">
         <v>40.61</v>
-      </c>
-      <c r="O30">
-        <v>1.4750000000000001</v>
       </c>
       <c r="P30">
         <v>0.1</v>
       </c>
       <c r="Q30">
+        <v>1.4750000000000001</v>
+      </c>
+      <c r="R30">
         <v>1.56</v>
       </c>
-      <c r="R30">
+      <c r="S30">
         <v>1.39</v>
       </c>
-      <c r="S30">
+      <c r="T30">
         <v>26.06</v>
       </c>
-      <c r="T30">
+      <c r="U30">
         <v>3.653144138</v>
       </c>
-      <c r="U30">
+      <c r="V30">
         <v>0.277361319</v>
       </c>
-      <c r="V30">
+      <c r="W30">
         <v>8.0842412360000004</v>
       </c>
-      <c r="W30">
+      <c r="X30">
         <v>7.0234279309999996</v>
       </c>
-      <c r="X30">
+      <c r="Y30">
         <v>0.66700000000000004</v>
-      </c>
-      <c r="Y30">
-        <v>0.66</v>
       </c>
       <c r="Z30">
         <v>1.4977</v>
       </c>
       <c r="AA30" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="AB30" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B31" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -3623,13 +3653,13 @@
         <v>1</v>
       </c>
       <c r="I31">
-        <v>1</v>
+        <v>0.495</v>
       </c>
       <c r="J31">
-        <v>0.39600000000000002</v>
+        <v>1</v>
       </c>
       <c r="K31" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L31">
         <v>1</v>
@@ -3638,57 +3668,57 @@
         <v>8</v>
       </c>
       <c r="N31">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="O31">
         <v>38.06</v>
-      </c>
-      <c r="O31">
-        <v>2.4449999999999998</v>
       </c>
       <c r="P31">
         <v>0.17</v>
       </c>
       <c r="Q31">
+        <v>2.4449999999999998</v>
+      </c>
+      <c r="R31">
         <v>2.5099999999999998</v>
       </c>
-      <c r="R31">
+      <c r="S31">
         <v>2.38</v>
       </c>
-      <c r="S31">
+      <c r="T31">
         <v>15.15</v>
       </c>
-      <c r="T31">
+      <c r="U31">
         <v>1.366512231</v>
       </c>
-      <c r="U31">
+      <c r="V31">
         <v>0.270114943</v>
       </c>
-      <c r="V31">
+      <c r="W31">
         <v>13.68183333</v>
       </c>
-      <c r="W31">
+      <c r="X31">
         <v>13.986743880000001</v>
       </c>
-      <c r="X31">
+      <c r="Y31">
         <v>0.17399999999999999</v>
-      </c>
-      <c r="Y31">
-        <v>0.495</v>
       </c>
       <c r="Z31">
         <v>0.61839999999999995</v>
       </c>
       <c r="AA31" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="AB31" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B32" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -3709,13 +3739,13 @@
         <v>1</v>
       </c>
       <c r="I32">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="J32">
-        <v>1.2330000000000001</v>
+        <v>1</v>
       </c>
       <c r="K32" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L32">
         <v>0.83333333300000001</v>
@@ -3724,57 +3754,57 @@
         <v>9</v>
       </c>
       <c r="N32">
+        <v>1.2330000000000001</v>
+      </c>
+      <c r="O32">
         <v>42.88</v>
-      </c>
-      <c r="O32">
-        <v>1.44</v>
       </c>
       <c r="P32">
         <v>0.15</v>
       </c>
       <c r="Q32">
+        <v>1.44</v>
+      </c>
+      <c r="R32">
         <v>1.48</v>
       </c>
-      <c r="R32">
+      <c r="S32">
         <v>1.4</v>
       </c>
-      <c r="S32">
+      <c r="T32">
         <v>28.95</v>
       </c>
-      <c r="T32">
+      <c r="U32">
         <v>3.5669515020000002</v>
       </c>
-      <c r="U32">
+      <c r="V32">
         <v>0.289230769</v>
       </c>
-      <c r="V32">
+      <c r="W32">
         <v>8.133336774</v>
       </c>
-      <c r="W32">
+      <c r="X32">
         <v>6.8565242489999996</v>
       </c>
-      <c r="X32">
+      <c r="Y32">
         <v>0.65</v>
-      </c>
-      <c r="Y32">
-        <v>0.6</v>
       </c>
       <c r="Z32">
         <v>1.4922</v>
       </c>
       <c r="AA32" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="AB32" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B33" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -3795,13 +3825,13 @@
         <v>0</v>
       </c>
       <c r="I33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J33">
-        <v>1.423</v>
+        <v>0</v>
       </c>
       <c r="K33" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L33">
         <v>2.3333333330000001</v>
@@ -3810,57 +3840,57 @@
         <v>5</v>
       </c>
       <c r="N33">
+        <v>1.423</v>
+      </c>
+      <c r="O33">
         <v>46.06</v>
-      </c>
-      <c r="O33">
-        <v>1.95</v>
       </c>
       <c r="P33">
         <v>0.2</v>
       </c>
       <c r="Q33">
+        <v>1.95</v>
+      </c>
+      <c r="R33">
         <v>2.06</v>
       </c>
-      <c r="R33">
+      <c r="S33">
         <v>1.84</v>
       </c>
-      <c r="S33">
+      <c r="T33">
         <v>22.39</v>
       </c>
-      <c r="T33">
+      <c r="U33">
         <v>5.0063417680000004</v>
       </c>
-      <c r="U33">
+      <c r="V33">
         <v>0.34204793</v>
       </c>
-      <c r="V33">
+      <c r="W33">
         <v>14.66934313</v>
       </c>
-      <c r="W33">
+      <c r="X33">
         <v>9.196829116</v>
       </c>
-      <c r="X33">
+      <c r="Y33">
         <v>0.91800000000000004</v>
-      </c>
-      <c r="Y33">
-        <v>1</v>
       </c>
       <c r="Z33">
         <v>4.5768000000000004</v>
       </c>
       <c r="AA33" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="AB33" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B34" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -3881,13 +3911,13 @@
         <v>1</v>
       </c>
       <c r="I34">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="J34">
-        <v>1.998</v>
+        <v>0</v>
       </c>
       <c r="K34" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L34">
         <v>3</v>
@@ -3896,57 +3926,57 @@
         <v>6</v>
       </c>
       <c r="N34">
+        <v>1.998</v>
+      </c>
+      <c r="O34">
         <v>46.2</v>
-      </c>
-      <c r="O34">
-        <v>1.54</v>
       </c>
       <c r="P34">
         <v>0.14000000000000001</v>
       </c>
       <c r="Q34">
+        <v>1.54</v>
+      </c>
+      <c r="R34">
         <v>1.58</v>
       </c>
-      <c r="R34">
+      <c r="S34">
         <v>1.5</v>
       </c>
-      <c r="S34">
+      <c r="T34">
         <v>29.16</v>
       </c>
-      <c r="T34">
+      <c r="U34">
         <v>14.20687212</v>
       </c>
-      <c r="U34">
+      <c r="V34">
         <v>0.35143288099999997</v>
       </c>
-      <c r="V34">
+      <c r="W34">
         <v>10.6774091</v>
       </c>
-      <c r="W34">
+      <c r="X34">
         <v>2.1365639399999998</v>
       </c>
-      <c r="X34">
+      <c r="Y34">
         <v>0.66300000000000003</v>
-      </c>
-      <c r="Y34">
-        <v>0.8</v>
       </c>
       <c r="Z34">
         <v>2.3984999999999999</v>
       </c>
       <c r="AA34" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="AB34" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B35" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -3967,13 +3997,13 @@
         <v>1</v>
       </c>
       <c r="I35">
-        <v>0</v>
+        <v>0.91300000000000003</v>
       </c>
       <c r="J35">
-        <v>1.083</v>
+        <v>0</v>
       </c>
       <c r="K35" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L35">
         <v>2</v>
@@ -3982,57 +4012,57 @@
         <v>18</v>
       </c>
       <c r="N35">
+        <v>1.083</v>
+      </c>
+      <c r="O35">
         <v>47.45</v>
-      </c>
-      <c r="O35">
-        <v>1.71</v>
       </c>
       <c r="P35">
         <v>0.15</v>
       </c>
       <c r="Q35">
+        <v>1.71</v>
+      </c>
+      <c r="R35">
         <v>1.79</v>
       </c>
-      <c r="R35">
+      <c r="S35">
         <v>1.63</v>
       </c>
-      <c r="S35">
+      <c r="T35">
         <v>26.53</v>
       </c>
-      <c r="T35">
+      <c r="U35">
         <v>3.9246911000000002E-2</v>
       </c>
-      <c r="U35">
+      <c r="V35">
         <v>0.44444444399999999</v>
       </c>
-      <c r="V35">
+      <c r="W35">
         <v>11.85616667</v>
       </c>
-      <c r="W35">
+      <c r="X35">
         <v>10.24037654</v>
       </c>
-      <c r="X35">
+      <c r="Y35">
         <v>0.153</v>
-      </c>
-      <c r="Y35">
-        <v>0.91300000000000003</v>
       </c>
       <c r="Z35">
         <v>0.74590000000000001</v>
       </c>
       <c r="AA35" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="AB35" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B36" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -4053,13 +4083,13 @@
         <v>0</v>
       </c>
       <c r="I36">
-        <v>0</v>
+        <v>0.82699999999999996</v>
       </c>
       <c r="J36">
-        <v>0.40300000000000002</v>
+        <v>0</v>
       </c>
       <c r="K36" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L36">
         <v>1.6666666670000001</v>
@@ -4068,57 +4098,57 @@
         <v>5</v>
       </c>
       <c r="N36">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="O36">
         <v>42.24</v>
-      </c>
-      <c r="O36">
-        <v>2.8050000000000002</v>
       </c>
       <c r="P36">
         <v>0.19</v>
       </c>
       <c r="Q36">
+        <v>2.8050000000000002</v>
+      </c>
+      <c r="R36">
         <v>2.93</v>
       </c>
-      <c r="R36">
+      <c r="S36">
         <v>2.68</v>
       </c>
-      <c r="S36">
+      <c r="T36">
         <v>14.42</v>
       </c>
-      <c r="T36">
+      <c r="U36">
         <v>8.1864801000000001E-2</v>
       </c>
-      <c r="U36">
+      <c r="V36">
         <v>0.30612244900000002</v>
       </c>
-      <c r="V36">
+      <c r="W36">
         <v>12.3225</v>
       </c>
-      <c r="W36">
+      <c r="X36">
         <v>16.789067599999999</v>
       </c>
-      <c r="X36">
+      <c r="Y36">
         <v>9.8000000000000004E-2</v>
-      </c>
-      <c r="Y36">
-        <v>0.82699999999999996</v>
       </c>
       <c r="Z36">
         <v>0.35670000000000002</v>
       </c>
       <c r="AA36" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="AB36" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B37" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -4139,13 +4169,13 @@
         <v>0</v>
       </c>
       <c r="I37">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="J37">
-        <v>0.158</v>
+        <v>1</v>
       </c>
       <c r="K37" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L37">
         <v>1.6666666670000001</v>
@@ -4154,57 +4184,57 @@
         <v>8</v>
       </c>
       <c r="N37">
+        <v>0.158</v>
+      </c>
+      <c r="O37">
         <v>43.26</v>
-      </c>
-      <c r="O37">
-        <v>1.4650000000000001</v>
       </c>
       <c r="P37">
         <v>0.13</v>
       </c>
       <c r="Q37">
+        <v>1.4650000000000001</v>
+      </c>
+      <c r="R37">
         <v>1.53</v>
       </c>
-      <c r="R37">
+      <c r="S37">
         <v>1.4</v>
       </c>
-      <c r="S37">
+      <c r="T37">
         <v>28.34</v>
       </c>
-      <c r="T37">
+      <c r="U37">
         <v>0.33945801599999997</v>
       </c>
-      <c r="U37">
+      <c r="V37">
         <v>0.37012987000000003</v>
       </c>
-      <c r="V37">
+      <c r="W37">
         <v>14.204404759999999</v>
       </c>
-      <c r="W37">
+      <c r="X37">
         <v>8.620270992</v>
       </c>
-      <c r="X37">
+      <c r="Y37">
         <v>0.154</v>
-      </c>
-      <c r="Y37">
-        <v>0.9</v>
       </c>
       <c r="Z37">
         <v>0.81930000000000003</v>
       </c>
       <c r="AA37" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="AB37" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B38" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -4225,13 +4255,13 @@
         <v>1</v>
       </c>
       <c r="I38">
-        <v>0</v>
+        <v>0.745</v>
       </c>
       <c r="J38">
-        <v>1.5149999999999999</v>
+        <v>0</v>
       </c>
       <c r="K38" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L38">
         <v>3</v>
@@ -4240,57 +4270,57 @@
         <v>11</v>
       </c>
       <c r="N38">
+        <v>1.5149999999999999</v>
+      </c>
+      <c r="O38">
         <v>42.11</v>
-      </c>
-      <c r="O38">
-        <v>2.0299999999999998</v>
       </c>
       <c r="P38">
         <v>0.09</v>
       </c>
       <c r="Q38">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="R38">
         <v>2.11</v>
       </c>
-      <c r="R38">
+      <c r="S38">
         <v>1.95</v>
       </c>
-      <c r="S38">
+      <c r="T38">
         <v>20</v>
       </c>
-      <c r="T38">
+      <c r="U38">
         <v>3.5732717799999998</v>
       </c>
-      <c r="U38">
+      <c r="V38">
         <v>0.38426349500000001</v>
       </c>
-      <c r="V38">
+      <c r="W38">
         <v>9.8117718479999994</v>
       </c>
-      <c r="W38">
+      <c r="X38">
         <v>10.39336411</v>
       </c>
-      <c r="X38">
+      <c r="Y38">
         <v>1.093</v>
-      </c>
-      <c r="Y38">
-        <v>0.745</v>
       </c>
       <c r="Z38">
         <v>3.9287999999999998</v>
       </c>
       <c r="AA38" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="AB38" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B39" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -4311,13 +4341,13 @@
         <v>0</v>
       </c>
       <c r="I39">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="J39">
-        <v>0.79300000000000004</v>
+        <v>0</v>
       </c>
       <c r="K39" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L39">
         <v>1</v>
@@ -4326,57 +4356,57 @@
         <v>5</v>
       </c>
       <c r="N39">
+        <v>0.79300000000000004</v>
+      </c>
+      <c r="O39">
         <v>45.04</v>
-      </c>
-      <c r="O39">
-        <v>2.0350000000000001</v>
       </c>
       <c r="P39">
         <v>0.15</v>
       </c>
       <c r="Q39">
+        <v>2.0350000000000001</v>
+      </c>
+      <c r="R39">
         <v>2.13</v>
       </c>
-      <c r="R39">
+      <c r="S39">
         <v>1.94</v>
       </c>
-      <c r="S39">
+      <c r="T39">
         <v>21.11</v>
       </c>
-      <c r="T39">
+      <c r="U39">
         <v>0.11334863100000001</v>
       </c>
-      <c r="U39">
+      <c r="V39">
         <v>0.30319148899999998</v>
       </c>
-      <c r="V39">
+      <c r="W39">
         <v>13.64392308</v>
       </c>
-      <c r="W39">
+      <c r="X39">
         <v>12.15332568</v>
       </c>
-      <c r="X39">
+      <c r="Y39">
         <v>0.188</v>
-      </c>
-      <c r="Y39">
-        <v>0.8</v>
       </c>
       <c r="Z39">
         <v>0.72760000000000002</v>
       </c>
       <c r="AA39" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="AB39" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B40" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -4397,13 +4427,13 @@
         <v>1</v>
       </c>
       <c r="I40">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="J40">
-        <v>2.1760000000000002</v>
+        <v>0</v>
       </c>
       <c r="K40" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L40">
         <v>1.3333333329999999</v>
@@ -4412,57 +4442,57 @@
         <v>16</v>
       </c>
       <c r="N40">
+        <v>2.1760000000000002</v>
+      </c>
+      <c r="O40">
         <v>48.13</v>
-      </c>
-      <c r="O40">
-        <v>1.95</v>
       </c>
       <c r="P40">
         <v>0.2</v>
       </c>
       <c r="Q40">
+        <v>1.95</v>
+      </c>
+      <c r="R40">
         <v>2.04</v>
       </c>
-      <c r="R40">
+      <c r="S40">
         <v>1.86</v>
       </c>
-      <c r="S40">
+      <c r="T40">
         <v>23.54</v>
       </c>
-      <c r="T40">
+      <c r="U40">
         <v>1.824014539</v>
       </c>
-      <c r="U40">
+      <c r="V40">
         <v>0.39895882599999999</v>
       </c>
-      <c r="V40">
+      <c r="W40">
         <v>9.0973486680000004</v>
       </c>
-      <c r="W40">
+      <c r="X40">
         <v>10.787992729999999</v>
       </c>
-      <c r="X40">
+      <c r="Y40">
         <v>2.113</v>
-      </c>
-      <c r="Y40">
-        <v>0.8</v>
       </c>
       <c r="Z40">
         <v>7.4108000000000001</v>
       </c>
       <c r="AA40" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="AB40" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B41" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -4483,13 +4513,13 @@
         <v>0</v>
       </c>
       <c r="I41">
-        <v>0</v>
+        <v>0.50800000000000001</v>
       </c>
       <c r="J41">
-        <v>3.3730000000000002</v>
+        <v>0</v>
       </c>
       <c r="K41" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L41">
         <v>2</v>
@@ -4498,57 +4528,57 @@
         <v>17</v>
       </c>
       <c r="N41">
+        <v>3.3730000000000002</v>
+      </c>
+      <c r="O41">
         <v>43</v>
-      </c>
-      <c r="O41">
-        <v>1.4650000000000001</v>
       </c>
       <c r="P41">
         <v>0.12</v>
       </c>
       <c r="Q41">
+        <v>1.4650000000000001</v>
+      </c>
+      <c r="R41">
         <v>1.54</v>
       </c>
-      <c r="R41">
+      <c r="S41">
         <v>1.39</v>
       </c>
-      <c r="S41">
+      <c r="T41">
         <v>27.97</v>
       </c>
-      <c r="T41">
+      <c r="U41">
         <v>0.711627495</v>
       </c>
-      <c r="U41">
+      <c r="V41">
         <v>0.28501827000000002</v>
       </c>
-      <c r="V41">
+      <c r="W41">
         <v>9.6740506869999994</v>
       </c>
-      <c r="W41">
+      <c r="X41">
         <v>8.434186253</v>
       </c>
-      <c r="X41">
+      <c r="Y41">
         <v>4.1050000000000004</v>
-      </c>
-      <c r="Y41">
-        <v>0.50800000000000001</v>
       </c>
       <c r="Z41">
         <v>11.0732</v>
       </c>
       <c r="AA41" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="AB41" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B42" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -4569,13 +4599,13 @@
         <v>1</v>
       </c>
       <c r="I42">
-        <v>1</v>
+        <v>0.71499999999999997</v>
       </c>
       <c r="J42">
-        <v>0.36099999999999999</v>
+        <v>1</v>
       </c>
       <c r="K42" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="L42">
         <v>2</v>
@@ -4584,57 +4614,57 @@
         <v>23</v>
       </c>
       <c r="N42">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="O42">
         <v>42.29</v>
-      </c>
-      <c r="O42">
-        <v>1.44</v>
       </c>
       <c r="P42">
         <v>0.09</v>
       </c>
       <c r="Q42">
+        <v>1.44</v>
+      </c>
+      <c r="R42">
         <v>1.52</v>
       </c>
-      <c r="R42">
+      <c r="S42">
         <v>1.36</v>
       </c>
-      <c r="S42">
+      <c r="T42">
         <v>27.88</v>
       </c>
-      <c r="T42">
+      <c r="U42">
         <v>0.81365362500000005</v>
       </c>
-      <c r="U42">
+      <c r="V42">
         <v>0.28947368400000001</v>
       </c>
-      <c r="V42">
+      <c r="W42">
         <v>16.863524200000001</v>
       </c>
-      <c r="W42">
+      <c r="X42">
         <v>8.2331731880000003</v>
       </c>
-      <c r="X42">
+      <c r="Y42">
         <v>0.64600000000000002</v>
-      </c>
-      <c r="Y42">
-        <v>0.71499999999999997</v>
       </c>
       <c r="Z42">
         <v>3.0055000000000001</v>
       </c>
       <c r="AA42" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="AB42" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="43" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B43" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -4655,13 +4685,13 @@
         <v>1</v>
       </c>
       <c r="I43">
-        <v>1</v>
+        <v>0.65</v>
       </c>
       <c r="J43">
-        <v>0.34300000000000003</v>
+        <v>1</v>
       </c>
       <c r="K43" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="L43">
         <v>1.5</v>
@@ -4670,57 +4700,57 @@
         <v>8</v>
       </c>
       <c r="N43">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="O43">
         <v>43.18</v>
-      </c>
-      <c r="O43">
-        <v>2.1549999999999998</v>
       </c>
       <c r="P43">
         <v>0.12</v>
       </c>
       <c r="Q43">
+        <v>2.1549999999999998</v>
+      </c>
+      <c r="R43">
         <v>2.23</v>
       </c>
-      <c r="R43">
+      <c r="S43">
         <v>2.08</v>
       </c>
-      <c r="S43">
+      <c r="T43">
         <v>19.32</v>
       </c>
-      <c r="T43">
+      <c r="U43">
         <v>3.2081617659999999</v>
       </c>
-      <c r="U43">
+      <c r="V43">
         <v>0.41767068299999999</v>
       </c>
-      <c r="V43">
+      <c r="W43">
         <v>10.968804220000001</v>
       </c>
-      <c r="W43">
+      <c r="X43">
         <v>11.32591912</v>
       </c>
-      <c r="X43">
+      <c r="Y43">
         <v>0.249</v>
-      </c>
-      <c r="Y43">
-        <v>0.65</v>
       </c>
       <c r="Z43">
         <v>1.0808</v>
       </c>
       <c r="AA43" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="AB43" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B44" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -4741,13 +4771,13 @@
         <v>1</v>
       </c>
       <c r="I44">
-        <v>0</v>
+        <v>0.85699999999999998</v>
       </c>
       <c r="J44">
-        <v>2.7509999999999999</v>
+        <v>0</v>
       </c>
       <c r="K44" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L44">
         <v>2.3333333330000001</v>
@@ -4756,57 +4786,57 @@
         <v>10</v>
       </c>
       <c r="N44">
+        <v>2.7509999999999999</v>
+      </c>
+      <c r="O44">
         <v>45.76</v>
-      </c>
-      <c r="O44">
-        <v>2.08</v>
       </c>
       <c r="P44">
         <v>0.12</v>
       </c>
       <c r="Q44">
+        <v>2.08</v>
+      </c>
+      <c r="R44">
         <v>2.17</v>
       </c>
-      <c r="R44">
+      <c r="S44">
         <v>1.99</v>
       </c>
-      <c r="S44">
+      <c r="T44">
         <v>21.13</v>
       </c>
-      <c r="T44">
+      <c r="U44">
         <v>0.30334931199999998</v>
       </c>
-      <c r="U44">
+      <c r="V44">
         <v>0.34765625</v>
       </c>
-      <c r="V44">
+      <c r="W44">
         <v>8.6619870989999992</v>
       </c>
-      <c r="W44">
+      <c r="X44">
         <v>12.328325339999999</v>
       </c>
-      <c r="X44">
+      <c r="Y44">
         <v>0.76800000000000002</v>
-      </c>
-      <c r="Y44">
-        <v>0.85699999999999998</v>
       </c>
       <c r="Z44">
         <v>2.1073</v>
       </c>
       <c r="AA44" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AB44" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B45" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -4827,13 +4857,13 @@
         <v>0</v>
       </c>
       <c r="I45">
-        <v>0</v>
+        <v>0.87</v>
       </c>
       <c r="J45">
-        <v>0.57999999999999996</v>
+        <v>0</v>
       </c>
       <c r="K45" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L45">
         <v>2</v>
@@ -4842,57 +4872,57 @@
         <v>15</v>
       </c>
       <c r="N45">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="O45">
         <v>42.34</v>
-      </c>
-      <c r="O45">
-        <v>1.625</v>
       </c>
       <c r="P45">
         <v>0.26</v>
       </c>
       <c r="Q45">
+        <v>1.625</v>
+      </c>
+      <c r="R45">
         <v>1.69</v>
       </c>
-      <c r="R45">
+      <c r="S45">
         <v>1.56</v>
       </c>
-      <c r="S45">
+      <c r="T45">
         <v>25.06</v>
       </c>
-      <c r="T45">
+      <c r="U45">
         <v>0.33709182700000001</v>
       </c>
-      <c r="U45">
+      <c r="V45">
         <v>0.48453608199999998</v>
       </c>
-      <c r="V45">
+      <c r="W45">
         <v>12.59883333</v>
       </c>
-      <c r="W45">
+      <c r="X45">
         <v>9.5814540869999991</v>
       </c>
-      <c r="X45">
+      <c r="Y45">
         <v>9.7000000000000003E-2</v>
-      </c>
-      <c r="Y45">
-        <v>0.87</v>
       </c>
       <c r="Z45">
         <v>0.58840000000000003</v>
       </c>
       <c r="AA45" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="AB45" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B46" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -4913,13 +4943,13 @@
         <v>1</v>
       </c>
       <c r="I46">
-        <v>0</v>
+        <v>0.96399999999999997</v>
       </c>
       <c r="J46">
-        <v>0.86399999999999999</v>
+        <v>0</v>
       </c>
       <c r="K46" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L46">
         <v>0.83333333300000001</v>
@@ -4928,57 +4958,57 @@
         <v>9</v>
       </c>
       <c r="N46">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="O46">
         <v>45.34</v>
-      </c>
-      <c r="O46">
-        <v>2.2000000000000002</v>
       </c>
       <c r="P46">
         <v>0.2</v>
       </c>
       <c r="Q46">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="R46">
         <v>2.2599999999999998</v>
       </c>
-      <c r="R46">
+      <c r="S46">
         <v>2.14</v>
       </c>
-      <c r="S46">
+      <c r="T46">
         <v>20.09</v>
       </c>
-      <c r="T46">
+      <c r="U46">
         <v>1.59382764</v>
       </c>
-      <c r="U46">
+      <c r="V46">
         <v>0.33124999999999999</v>
       </c>
-      <c r="V46">
+      <c r="W46">
         <v>16.15370635</v>
       </c>
-      <c r="W46">
+      <c r="X46">
         <v>12.403086180000001</v>
       </c>
-      <c r="X46">
+      <c r="Y46">
         <v>0.16</v>
-      </c>
-      <c r="Y46">
-        <v>0.96399999999999997</v>
       </c>
       <c r="Z46">
         <v>0.86209999999999998</v>
       </c>
       <c r="AA46" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="AB46" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B47" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -4999,13 +5029,13 @@
         <v>1</v>
       </c>
       <c r="I47">
-        <v>0</v>
+        <v>0.50800000000000001</v>
       </c>
       <c r="J47">
-        <v>2.5569999999999999</v>
+        <v>0</v>
       </c>
       <c r="K47" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L47">
         <v>3</v>
@@ -5014,57 +5044,57 @@
         <v>10</v>
       </c>
       <c r="N47">
+        <v>2.5569999999999999</v>
+      </c>
+      <c r="O47">
         <v>43.84</v>
-      </c>
-      <c r="O47">
-        <v>2.46</v>
       </c>
       <c r="P47">
         <v>0.17</v>
       </c>
       <c r="Q47">
+        <v>2.46</v>
+      </c>
+      <c r="R47">
         <v>2.59</v>
       </c>
-      <c r="R47">
+      <c r="S47">
         <v>2.33</v>
       </c>
-      <c r="S47">
+      <c r="T47">
         <v>16.93</v>
       </c>
-      <c r="T47">
+      <c r="U47">
         <v>1.384743681</v>
       </c>
-      <c r="U47">
+      <c r="V47">
         <v>0.22228637400000001</v>
       </c>
-      <c r="V47">
+      <c r="W47">
         <v>16.741183039999999</v>
       </c>
-      <c r="W47">
+      <c r="X47">
         <v>14.06762816</v>
       </c>
-      <c r="X47">
+      <c r="Y47">
         <v>1.732</v>
-      </c>
-      <c r="Y47">
-        <v>0.50800000000000001</v>
       </c>
       <c r="Z47">
         <v>5.9958</v>
       </c>
       <c r="AA47" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="AB47" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="48" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B48" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -5085,13 +5115,13 @@
         <v>0</v>
       </c>
       <c r="I48">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="J48">
-        <v>0.47099999999999997</v>
+        <v>1</v>
       </c>
       <c r="K48" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="L48">
         <v>1.3333333329999999</v>
@@ -5100,57 +5130,57 @@
         <v>10</v>
       </c>
       <c r="N48">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="O48">
         <v>41.64</v>
-      </c>
-      <c r="O48">
-        <v>2.0449999999999999</v>
       </c>
       <c r="P48">
         <v>0.15</v>
       </c>
       <c r="Q48">
+        <v>2.0449999999999999</v>
+      </c>
+      <c r="R48">
         <v>2.17</v>
       </c>
-      <c r="R48">
+      <c r="S48">
         <v>1.92</v>
       </c>
-      <c r="S48">
+      <c r="T48">
         <v>19.23</v>
       </c>
-      <c r="T48">
+      <c r="U48">
         <v>5.4886813999999999E-2</v>
       </c>
-      <c r="U48">
+      <c r="V48">
         <v>0.30442804400000001</v>
       </c>
-      <c r="V48">
+      <c r="W48">
         <v>13.17430738</v>
       </c>
-      <c r="W48">
+      <c r="X48">
         <v>12.24255659</v>
       </c>
-      <c r="X48">
+      <c r="Y48">
         <v>0.54200000000000004</v>
-      </c>
-      <c r="Y48">
-        <v>0.9</v>
       </c>
       <c r="Z48">
         <v>2.1572</v>
       </c>
       <c r="AA48" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="AB48" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="49" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B49" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -5171,13 +5201,13 @@
         <v>0</v>
       </c>
       <c r="I49">
-        <v>1</v>
+        <v>0.75800000000000001</v>
       </c>
       <c r="J49">
-        <v>0.42199999999999999</v>
+        <v>1</v>
       </c>
       <c r="K49" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="L49">
         <v>1.6666666670000001</v>
@@ -5186,57 +5216,60 @@
         <v>9</v>
       </c>
       <c r="N49">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="O49">
         <v>42.85</v>
-      </c>
-      <c r="O49">
-        <v>2.5049999999999999</v>
       </c>
       <c r="P49">
         <v>0.2</v>
       </c>
       <c r="Q49">
+        <v>2.5049999999999999</v>
+      </c>
+      <c r="R49">
         <v>2.61</v>
       </c>
-      <c r="R49">
+      <c r="S49">
         <v>2.4</v>
       </c>
-      <c r="S49">
+      <c r="T49">
         <v>16.41</v>
       </c>
-      <c r="T49">
+      <c r="U49">
         <v>0.40545273399999998</v>
       </c>
-      <c r="U49">
+      <c r="V49">
         <v>0.274074074</v>
       </c>
-      <c r="V49">
+      <c r="W49">
         <v>17.785309519999998</v>
       </c>
-      <c r="W49">
+      <c r="X49">
         <v>14.827273630000001</v>
       </c>
-      <c r="X49">
+      <c r="Y49">
         <v>0.27</v>
-      </c>
-      <c r="Y49">
-        <v>0.75800000000000001</v>
       </c>
       <c r="Z49">
         <v>1.28</v>
       </c>
       <c r="AA49" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="AB49" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
+  <conditionalFormatting sqref="AC10:AC11">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC10:AC11">
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>